<commit_message>
fixed issue in safety feature that consists of attacks on civilians and was not computed per head before; also recreated dataset without flight data
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -639,16 +639,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="D2" t="n">
         <v>3.9</v>
       </c>
       <c r="E2" t="n">
-        <v>10.1</v>
+        <v>9.5</v>
       </c>
       <c r="F2" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -659,16 +659,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="D3" t="n">
         <v>3.7</v>
       </c>
       <c r="E3" t="n">
-        <v>10.5</v>
+        <v>9.9</v>
       </c>
       <c r="F3" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -679,16 +679,16 @@
         <v>0.3</v>
       </c>
       <c r="C4" t="n">
-        <v>6.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4" t="n">
         <v>1.8</v>
       </c>
       <c r="E4" t="n">
-        <v>8.5</v>
+        <v>2.6</v>
       </c>
       <c r="F4" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -699,16 +699,16 @@
         <v>0.4</v>
       </c>
       <c r="C5" t="n">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="D5" t="n">
         <v>1.6</v>
       </c>
       <c r="E5" t="n">
-        <v>8.4</v>
+        <v>7.5</v>
       </c>
       <c r="F5" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -719,16 +719,16 @@
         <v>0.8</v>
       </c>
       <c r="C6" t="n">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -739,16 +739,16 @@
         <v>0.8</v>
       </c>
       <c r="C7" t="n">
-        <v>1.1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" t="n">
         <v>6.5</v>
       </c>
       <c r="E7" t="n">
-        <v>8.4</v>
+        <v>7.8</v>
       </c>
       <c r="F7" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -759,16 +759,16 @@
         <v>0.9</v>
       </c>
       <c r="C8" t="n">
-        <v>6.2</v>
+        <v>4.9</v>
       </c>
       <c r="D8" t="n">
         <v>1.2</v>
       </c>
       <c r="E8" t="n">
-        <v>8.300000000000001</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -779,16 +779,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>4.1</v>
+        <v>5.3</v>
       </c>
       <c r="D9" t="n">
         <v>6.5</v>
       </c>
       <c r="E9" t="n">
-        <v>11.6</v>
+        <v>12.8</v>
       </c>
       <c r="F9" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -799,16 +799,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>5.9</v>
       </c>
       <c r="D10" t="n">
         <v>3.4</v>
       </c>
       <c r="E10" t="n">
-        <v>8.4</v>
+        <v>10.3</v>
       </c>
       <c r="F10" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -819,16 +819,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="D11" t="n">
         <v>5.3</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="F11" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -839,16 +839,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>6.4</v>
+        <v>5.1</v>
       </c>
       <c r="D12" t="n">
         <v>5.2</v>
       </c>
       <c r="E12" t="n">
-        <v>12.6</v>
+        <v>11.3</v>
       </c>
       <c r="F12" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -859,16 +859,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="D13" t="n">
         <v>5.4</v>
       </c>
       <c r="E13" t="n">
-        <v>12.4</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -879,16 +879,16 @@
         <v>1.1</v>
       </c>
       <c r="C14" t="n">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="D14" t="n">
         <v>4.5</v>
       </c>
       <c r="E14" t="n">
-        <v>12.2</v>
+        <v>11.8</v>
       </c>
       <c r="F14" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -899,16 +899,16 @@
         <v>1.2</v>
       </c>
       <c r="C15" t="n">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="D15" t="n">
         <v>0.2</v>
       </c>
       <c r="E15" t="n">
-        <v>8.1</v>
+        <v>7.5</v>
       </c>
       <c r="F15" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -919,16 +919,16 @@
         <v>1.4</v>
       </c>
       <c r="C16" t="n">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="D16" t="n">
         <v>4.7</v>
       </c>
       <c r="E16" t="n">
-        <v>11.6</v>
+        <v>12.2</v>
       </c>
       <c r="F16" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -939,16 +939,16 @@
         <v>1.8</v>
       </c>
       <c r="C17" t="n">
-        <v>1.2</v>
+        <v>5.4</v>
       </c>
       <c r="D17" t="n">
         <v>5.8</v>
       </c>
       <c r="E17" t="n">
-        <v>8.800000000000001</v>
+        <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -959,16 +959,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>3.9</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
         <v>6.2</v>
       </c>
       <c r="E18" t="n">
-        <v>12.1</v>
+        <v>14.2</v>
       </c>
       <c r="F18" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -979,16 +979,16 @@
         <v>2.2</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="D19" t="n">
         <v>6.8</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>14.4</v>
       </c>
       <c r="F19" t="n">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -999,16 +999,16 @@
         <v>2.2</v>
       </c>
       <c r="C20" t="n">
-        <v>4.1</v>
+        <v>5.6</v>
       </c>
       <c r="D20" t="n">
         <v>5.8</v>
       </c>
       <c r="E20" t="n">
-        <v>12.1</v>
+        <v>13.6</v>
       </c>
       <c r="F20" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1019,16 +1019,16 @@
         <v>2.4</v>
       </c>
       <c r="C21" t="n">
-        <v>6.8</v>
+        <v>3.9</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>9.199999999999999</v>
+        <v>6.3</v>
       </c>
       <c r="F21" t="n">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1039,16 +1039,16 @@
         <v>3.3</v>
       </c>
       <c r="C22" t="n">
-        <v>5.9</v>
+        <v>2.7</v>
       </c>
       <c r="D22" t="n">
         <v>3.7</v>
       </c>
       <c r="E22" t="n">
-        <v>12.9</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1059,16 +1059,16 @@
         <v>3.7</v>
       </c>
       <c r="C23" t="n">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="D23" t="n">
         <v>0.9</v>
       </c>
       <c r="E23" t="n">
-        <v>10.8</v>
+        <v>10.3</v>
       </c>
       <c r="F23" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1079,16 +1079,16 @@
         <v>3.9</v>
       </c>
       <c r="C24" t="n">
-        <v>2.3</v>
+        <v>5.3</v>
       </c>
       <c r="D24" t="n">
         <v>2.3</v>
       </c>
       <c r="E24" t="n">
-        <v>8.5</v>
+        <v>11.5</v>
       </c>
       <c r="F24" t="n">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1099,16 +1099,16 @@
         <v>4.1</v>
       </c>
       <c r="C25" t="n">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="D25" t="n">
         <v>5.1</v>
       </c>
       <c r="E25" t="n">
-        <v>16</v>
+        <v>15.3</v>
       </c>
       <c r="F25" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1119,16 +1119,16 @@
         <v>4.2</v>
       </c>
       <c r="C26" t="n">
-        <v>6.5</v>
+        <v>3.6</v>
       </c>
       <c r="D26" t="n">
         <v>0.4</v>
       </c>
       <c r="E26" t="n">
-        <v>11.1</v>
+        <v>8.200000000000001</v>
       </c>
       <c r="F26" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1139,16 +1139,16 @@
         <v>4.2</v>
       </c>
       <c r="C27" t="n">
-        <v>6.4</v>
+        <v>5.7</v>
       </c>
       <c r="D27" t="n">
         <v>6.7</v>
       </c>
       <c r="E27" t="n">
-        <v>17.3</v>
+        <v>16.6</v>
       </c>
       <c r="F27" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1159,16 +1159,16 @@
         <v>4.3</v>
       </c>
       <c r="C28" t="n">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>7.699999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="F28" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1179,16 +1179,16 @@
         <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="D29" t="n">
         <v>3.9</v>
       </c>
       <c r="E29" t="n">
-        <v>15.6</v>
+        <v>15</v>
       </c>
       <c r="F29" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1199,16 +1199,16 @@
         <v>5.1</v>
       </c>
       <c r="C30" t="n">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
         <v>6.6</v>
       </c>
       <c r="E30" t="n">
-        <v>17.9</v>
+        <v>17.7</v>
       </c>
       <c r="F30" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1219,16 +1219,16 @@
         <v>5.1</v>
       </c>
       <c r="C31" t="n">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="D31" t="n">
         <v>6.3</v>
       </c>
       <c r="E31" t="n">
-        <v>18.2</v>
+        <v>17.6</v>
       </c>
       <c r="F31" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1239,16 +1239,16 @@
         <v>5.2</v>
       </c>
       <c r="C32" t="n">
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="D32" t="n">
         <v>0.1</v>
       </c>
       <c r="E32" t="n">
-        <v>12</v>
+        <v>11.2</v>
       </c>
       <c r="F32" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1268,7 +1268,7 @@
         <v>18.8</v>
       </c>
       <c r="F33" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1279,16 +1279,16 @@
         <v>5.6</v>
       </c>
       <c r="C34" t="n">
-        <v>6.7</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
         <v>6</v>
       </c>
       <c r="E34" t="n">
-        <v>18.3</v>
+        <v>17.6</v>
       </c>
       <c r="F34" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1299,16 +1299,16 @@
         <v>5.8</v>
       </c>
       <c r="C35" t="n">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
       <c r="D35" t="n">
         <v>7.4</v>
       </c>
       <c r="E35" t="n">
-        <v>17.7</v>
+        <v>19.4</v>
       </c>
       <c r="F35" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1319,16 +1319,16 @@
         <v>6.1</v>
       </c>
       <c r="C36" t="n">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="D36" t="n">
         <v>4.6</v>
       </c>
       <c r="E36" t="n">
-        <v>16.8</v>
+        <v>16.3</v>
       </c>
       <c r="F36" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1339,16 +1339,16 @@
         <v>6.1</v>
       </c>
       <c r="C37" t="n">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="D37" t="n">
         <v>7.1</v>
       </c>
       <c r="E37" t="n">
-        <v>19.7</v>
+        <v>19.3</v>
       </c>
       <c r="F37" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1359,16 +1359,16 @@
         <v>6.2</v>
       </c>
       <c r="C38" t="n">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="D38" t="n">
         <v>5.9</v>
       </c>
       <c r="E38" t="n">
-        <v>18.9</v>
+        <v>18.2</v>
       </c>
       <c r="F38" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1379,16 +1379,16 @@
         <v>6.3</v>
       </c>
       <c r="C39" t="n">
-        <v>5.9</v>
+        <v>6.2</v>
       </c>
       <c r="D39" t="n">
         <v>6</v>
       </c>
       <c r="E39" t="n">
-        <v>18.2</v>
+        <v>18.5</v>
       </c>
       <c r="F39" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1399,16 +1399,16 @@
         <v>6.3</v>
       </c>
       <c r="C40" t="n">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="D40" t="n">
         <v>5.8</v>
       </c>
       <c r="E40" t="n">
-        <v>18.9</v>
+        <v>18.3</v>
       </c>
       <c r="F40" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1419,16 +1419,16 @@
         <v>6.4</v>
       </c>
       <c r="C41" t="n">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="D41" t="n">
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>19.7</v>
+        <v>19.6</v>
       </c>
       <c r="F41" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1439,16 +1439,16 @@
         <v>6.4</v>
       </c>
       <c r="C42" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="D42" t="n">
         <v>5.7</v>
       </c>
       <c r="E42" t="n">
-        <v>18.8</v>
+        <v>18.3</v>
       </c>
       <c r="F42" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1459,16 +1459,16 @@
         <v>6.4</v>
       </c>
       <c r="C43" t="n">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
         <v>6.9</v>
       </c>
       <c r="E43" t="n">
-        <v>19.9</v>
+        <v>19.3</v>
       </c>
       <c r="F43" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1479,16 +1479,16 @@
         <v>6.4</v>
       </c>
       <c r="C44" t="n">
-        <v>3.6</v>
+        <v>5.3</v>
       </c>
       <c r="D44" t="n">
         <v>5.8</v>
       </c>
       <c r="E44" t="n">
-        <v>15.8</v>
+        <v>17.5</v>
       </c>
       <c r="F44" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1499,16 +1499,16 @@
         <v>6.6</v>
       </c>
       <c r="C45" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="D45" t="n">
         <v>7.2</v>
       </c>
       <c r="E45" t="n">
-        <v>20.6</v>
+        <v>20.1</v>
       </c>
       <c r="F45" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1519,16 +1519,16 @@
         <v>6.7</v>
       </c>
       <c r="C46" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="D46" t="n">
         <v>7.4</v>
       </c>
       <c r="E46" t="n">
-        <v>20.9</v>
+        <v>20.4</v>
       </c>
       <c r="F46" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1548,7 +1548,7 @@
         <v>18.8</v>
       </c>
       <c r="F47" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1559,13 +1559,13 @@
         <v>6.9</v>
       </c>
       <c r="C48" t="n">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="D48" t="n">
         <v>6.1</v>
       </c>
       <c r="E48" t="n">
-        <v>18.8</v>
+        <v>19.1</v>
       </c>
       <c r="F48" t="n">
         <v>31</v>
@@ -1579,16 +1579,16 @@
         <v>6.9</v>
       </c>
       <c r="C49" t="n">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="D49" t="n">
         <v>7.5</v>
       </c>
       <c r="E49" t="n">
-        <v>21.1</v>
+        <v>20.7</v>
       </c>
       <c r="F49" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1599,13 +1599,13 @@
         <v>7</v>
       </c>
       <c r="C50" t="n">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
       <c r="D50" t="n">
         <v>4.7</v>
       </c>
       <c r="E50" t="n">
-        <v>16.4</v>
+        <v>17.4</v>
       </c>
       <c r="F50" t="n">
         <v>42</v>
@@ -1619,16 +1619,16 @@
         <v>7</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="D51" t="n">
         <v>7.4</v>
       </c>
       <c r="E51" t="n">
-        <v>14.4</v>
+        <v>20.6</v>
       </c>
       <c r="F51" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1639,16 +1639,16 @@
         <v>7</v>
       </c>
       <c r="C52" t="n">
-        <v>4.4</v>
+        <v>4.9</v>
       </c>
       <c r="D52" t="n">
         <v>7.3</v>
       </c>
       <c r="E52" t="n">
-        <v>18.7</v>
+        <v>19.2</v>
       </c>
       <c r="F52" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1659,16 +1659,16 @@
         <v>7.4</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9</v>
+        <v>5.5</v>
       </c>
       <c r="D53" t="n">
         <v>6.4</v>
       </c>
       <c r="E53" t="n">
-        <v>14.7</v>
+        <v>19.3</v>
       </c>
       <c r="F53" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1679,16 +1679,16 @@
         <v>7.5</v>
       </c>
       <c r="C54" t="n">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
         <v>3.7</v>
       </c>
       <c r="E54" t="n">
-        <v>17.8</v>
+        <v>17.2</v>
       </c>
       <c r="F54" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1699,16 +1699,16 @@
         <v>7.7</v>
       </c>
       <c r="C55" t="n">
-        <v>5.5</v>
+        <v>6.3</v>
       </c>
       <c r="D55" t="n">
         <v>7.4</v>
       </c>
       <c r="E55" t="n">
-        <v>20.6</v>
+        <v>21.4</v>
       </c>
       <c r="F55" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1719,16 +1719,16 @@
         <v>7.7</v>
       </c>
       <c r="C56" t="n">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="D56" t="n">
         <v>7.2</v>
       </c>
       <c r="E56" t="n">
-        <v>21.1</v>
+        <v>21</v>
       </c>
       <c r="F56" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1739,16 +1739,16 @@
         <v>7.8</v>
       </c>
       <c r="C57" t="n">
-        <v>4.3</v>
+        <v>6.1</v>
       </c>
       <c r="D57" t="n">
         <v>7.2</v>
       </c>
       <c r="E57" t="n">
-        <v>19.3</v>
+        <v>21.1</v>
       </c>
       <c r="F57" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1759,16 +1759,16 @@
         <v>7.9</v>
       </c>
       <c r="C58" t="n">
-        <v>5.3</v>
+        <v>6</v>
       </c>
       <c r="D58" t="n">
         <v>7.4</v>
       </c>
       <c r="E58" t="n">
-        <v>20.6</v>
+        <v>21.3</v>
       </c>
       <c r="F58" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1779,16 +1779,16 @@
         <v>8</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>2.9</v>
       </c>
       <c r="E59" t="n">
-        <v>11.7</v>
+        <v>10.9</v>
       </c>
       <c r="F59" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1799,16 +1799,16 @@
         <v>8.1</v>
       </c>
       <c r="C60" t="n">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="D60" t="n">
         <v>6.6</v>
       </c>
       <c r="E60" t="n">
-        <v>21.2</v>
+        <v>20.9</v>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1819,16 +1819,16 @@
         <v>8.1</v>
       </c>
       <c r="C61" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="D61" t="n">
         <v>7.3</v>
       </c>
       <c r="E61" t="n">
-        <v>22.2</v>
+        <v>21.7</v>
       </c>
       <c r="F61" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1839,16 +1839,16 @@
         <v>8.199999999999999</v>
       </c>
       <c r="C62" t="n">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
         <v>7.4</v>
       </c>
       <c r="E62" t="n">
-        <v>19</v>
+        <v>21.6</v>
       </c>
       <c r="F62" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1859,16 +1859,16 @@
         <v>8.300000000000001</v>
       </c>
       <c r="C63" t="n">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="D63" t="n">
         <v>7.3</v>
       </c>
       <c r="E63" t="n">
-        <v>22.2</v>
+        <v>21.9</v>
       </c>
       <c r="F63" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1879,16 +1879,16 @@
         <v>8.4</v>
       </c>
       <c r="C64" t="n">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="D64" t="n">
         <v>7.5</v>
       </c>
       <c r="E64" t="n">
-        <v>21.2</v>
+        <v>22.1</v>
       </c>
       <c r="F64" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1899,13 +1899,13 @@
         <v>8.4</v>
       </c>
       <c r="C65" t="n">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="D65" t="n">
         <v>7.2</v>
       </c>
       <c r="E65" t="n">
-        <v>21.9</v>
+        <v>21.7</v>
       </c>
       <c r="F65" t="n">
         <v>7</v>
@@ -1919,16 +1919,16 @@
         <v>8.4</v>
       </c>
       <c r="C66" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="D66" t="n">
         <v>6.4</v>
       </c>
       <c r="E66" t="n">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="F66" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1939,16 +1939,16 @@
         <v>8.5</v>
       </c>
       <c r="C67" t="n">
-        <v>5.6</v>
+        <v>6.2</v>
       </c>
       <c r="D67" t="n">
         <v>6.7</v>
       </c>
       <c r="E67" t="n">
-        <v>20.8</v>
+        <v>21.4</v>
       </c>
       <c r="F67" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1959,16 +1959,16 @@
         <v>8.5</v>
       </c>
       <c r="C68" t="n">
-        <v>6.4</v>
+        <v>5</v>
       </c>
       <c r="D68" t="n">
         <v>6.2</v>
       </c>
       <c r="E68" t="n">
-        <v>21.1</v>
+        <v>19.7</v>
       </c>
       <c r="F68" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1979,13 +1979,13 @@
         <v>8.6</v>
       </c>
       <c r="C69" t="n">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="D69" t="n">
         <v>7.4</v>
       </c>
       <c r="E69" t="n">
-        <v>22.3</v>
+        <v>22.2</v>
       </c>
       <c r="F69" t="n">
         <v>3</v>
@@ -1999,16 +1999,16 @@
         <v>8.6</v>
       </c>
       <c r="C70" t="n">
-        <v>6.4</v>
+        <v>6.2</v>
       </c>
       <c r="D70" t="n">
         <v>7.4</v>
       </c>
       <c r="E70" t="n">
-        <v>22.4</v>
+        <v>22.2</v>
       </c>
       <c r="F70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2019,16 +2019,16 @@
         <v>8.6</v>
       </c>
       <c r="C71" t="n">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="D71" t="n">
         <v>7.4</v>
       </c>
       <c r="E71" t="n">
-        <v>22.7</v>
+        <v>22.3</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2039,16 +2039,16 @@
         <v>8.800000000000001</v>
       </c>
       <c r="C72" t="n">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="D72" t="n">
         <v>6.9</v>
       </c>
       <c r="E72" t="n">
-        <v>22</v>
+        <v>21.5</v>
       </c>
       <c r="F72" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2059,16 +2059,16 @@
         <v>9</v>
       </c>
       <c r="C73" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="D73" t="n">
         <v>5.9</v>
       </c>
       <c r="E73" t="n">
-        <v>21.6</v>
+        <v>21.1</v>
       </c>
       <c r="F73" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2079,16 +2079,16 @@
         <v>9.1</v>
       </c>
       <c r="C74" t="n">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="D74" t="n">
         <v>7.5</v>
       </c>
       <c r="E74" t="n">
-        <v>21.1</v>
+        <v>22.9</v>
       </c>
       <c r="F74" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2099,16 +2099,16 @@
         <v>9.199999999999999</v>
       </c>
       <c r="C75" t="n">
-        <v>4.2</v>
+        <v>5.8</v>
       </c>
       <c r="D75" t="n">
         <v>6.6</v>
       </c>
       <c r="E75" t="n">
-        <v>20</v>
+        <v>21.6</v>
       </c>
       <c r="F75" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>